<commit_message>
Row column count and check for any fields in row
</commit_message>
<xml_diff>
--- a/ProjectPOM/src/main/java/Resources/color.xlsx
+++ b/ProjectPOM/src/main/java/Resources/color.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25831"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\Desktop\java\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C23A9550-A9CA-408A-9C1B-17DC3937058C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E87EAD91-148E-4EEA-B073-8EFAFB661419}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Select Input" sheetId="1" r:id="rId1"/>
     <sheet name="Radio Buttons Demo" sheetId="2" r:id="rId2"/>
     <sheet name="Simple Form Demo" sheetId="3" r:id="rId3"/>
+    <sheet name="RowColumnTable" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="18">
   <si>
     <t>Red</t>
   </si>
@@ -68,13 +69,19 @@
     <t xml:space="preserve">Selected Color : </t>
   </si>
   <si>
-    <t xml:space="preserve">All selected colors are : </t>
-  </si>
-  <si>
     <t>Apple</t>
   </si>
   <si>
     <t>InputText</t>
+  </si>
+  <si>
+    <t>Sonya Frost Software Engineer Edinburgh 23 2008/12/13 $103,600</t>
+  </si>
+  <si>
+    <t>ExpectedField</t>
+  </si>
+  <si>
+    <t>All selected colors are : Green</t>
   </si>
 </sst>
 </file>
@@ -403,8 +410,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -434,7 +441,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
@@ -452,7 +459,7 @@
   <dimension ref="A1:A4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -490,7 +497,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5B0AE6C-C3CD-49FD-9C9C-AE3E72C377D1}">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
@@ -508,7 +515,7 @@
         <v>10</v>
       </c>
       <c r="C1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
@@ -519,7 +526,32 @@
         <v>11</v>
       </c>
       <c r="C2" t="s">
-        <v>14</v>
+        <v>13</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{14E3460F-51D7-4DBF-A806-B7ABE2EB0B53}">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Form submit data driven and parameters
</commit_message>
<xml_diff>
--- a/ProjectPOM/src/main/java/Resources/color.xlsx
+++ b/ProjectPOM/src/main/java/Resources/color.xlsx
@@ -8,15 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\Desktop\java\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E87EAD91-148E-4EEA-B073-8EFAFB661419}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D35AF7F5-6F13-40DC-A870-75BA0F23C67B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Select Input" sheetId="1" r:id="rId1"/>
-    <sheet name="Radio Buttons Demo" sheetId="2" r:id="rId2"/>
-    <sheet name="Simple Form Demo" sheetId="3" r:id="rId3"/>
-    <sheet name="RowColumnTable" sheetId="4" r:id="rId4"/>
+    <sheet name="FormSubmit" sheetId="5" r:id="rId2"/>
+    <sheet name="FormSubmitByParameter" sheetId="6" r:id="rId3"/>
+    <sheet name="FormSubmitByDataProvider" sheetId="7" r:id="rId4"/>
+    <sheet name="Radio Buttons Demo" sheetId="2" r:id="rId5"/>
+    <sheet name="Simple Form Demo" sheetId="3" r:id="rId6"/>
+    <sheet name="RowColumnTable" sheetId="4" r:id="rId7"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -28,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="31">
   <si>
     <t>Red</t>
   </si>
@@ -82,6 +85,45 @@
   </si>
   <si>
     <t>All selected colors are : Green</t>
+  </si>
+  <si>
+    <t>Sneha</t>
+  </si>
+  <si>
+    <t>Sneha95</t>
+  </si>
+  <si>
+    <t>George</t>
+  </si>
+  <si>
+    <t>Kottayam</t>
+  </si>
+  <si>
+    <t>Kerala</t>
+  </si>
+  <si>
+    <t>First Name</t>
+  </si>
+  <si>
+    <t>Last Name</t>
+  </si>
+  <si>
+    <t>UserName</t>
+  </si>
+  <si>
+    <t>City</t>
+  </si>
+  <si>
+    <t>State</t>
+  </si>
+  <si>
+    <t>Zip</t>
+  </si>
+  <si>
+    <t>Expected String</t>
+  </si>
+  <si>
+    <t>Form has been submitted successfully!</t>
   </si>
 </sst>
 </file>
@@ -410,7 +452,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -455,6 +497,111 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BEB26F93-AE3F-48A5-97B5-9D34F16AA0C7}">
+  <dimension ref="A1:F2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E2" t="s">
+        <v>22</v>
+      </c>
+      <c r="F2">
+        <v>698473</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD82844A-A525-4C73-AE33-C82C5F519403}">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF9CB2E8-2490-41FE-897C-5F845D977BF0}">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46FAF9C0-40A0-4810-AED5-87902B90760F}">
   <dimension ref="A1:A4"/>
   <sheetViews>
@@ -493,7 +640,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5B0AE6C-C3CD-49FD-9C9C-AE3E72C377D1}">
   <dimension ref="A1:C2"/>
   <sheetViews>
@@ -534,7 +681,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{14E3460F-51D7-4DBF-A806-B7ABE2EB0B53}">
   <dimension ref="A1:A2"/>
   <sheetViews>

</xml_diff>